<commit_message>
Fixing code and adding page object for all classes
</commit_message>
<xml_diff>
--- a/src/main/resources/DataProvider/contact_data_test.xlsx
+++ b/src/main/resources/DataProvider/contact_data_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Eclipse\WorkSpace\CRMTesting\lib\DataProvider\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Eclipse\WorkSpace\ClassicCRMTestMaven\src\main\resources\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Jsandye</t>
   </si>
@@ -79,57 +79,6 @@
   </si>
   <si>
     <t>Services</t>
-  </si>
-  <si>
-    <t>Clemence</t>
-  </si>
-  <si>
-    <t>Akred</t>
-  </si>
-  <si>
-    <t>Centidel</t>
-  </si>
-  <si>
-    <t>Legal</t>
-  </si>
-  <si>
-    <t>Mella</t>
-  </si>
-  <si>
-    <t>Duval</t>
-  </si>
-  <si>
-    <t>Aivee</t>
-  </si>
-  <si>
-    <t>Giacinta</t>
-  </si>
-  <si>
-    <t>Broadbere</t>
-  </si>
-  <si>
-    <t>Yakitri</t>
-  </si>
-  <si>
-    <t>Support</t>
-  </si>
-  <si>
-    <t>Welbie</t>
-  </si>
-  <si>
-    <t>Markey</t>
-  </si>
-  <si>
-    <t>Zoombox</t>
-  </si>
-  <si>
-    <t>Perry</t>
-  </si>
-  <si>
-    <t>Gozzard</t>
-  </si>
-  <si>
-    <t>Zooveo</t>
   </si>
 </sst>
 </file>
@@ -445,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -528,76 +477,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>